<commit_message>
Shyt-load of stuff to push to staging
</commit_message>
<xml_diff>
--- a/uploads/menu_file.xlsx
+++ b/uploads/menu_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmatr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58FB0D65-7E3F-4EA3-A4F6-51756B7E5EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F90374-943C-46CC-AF8F-D870DA54831D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="690" windowWidth="21600" windowHeight="11160" xr2:uid="{4EF278E9-0480-487F-AE82-D1D1DBD956EF}"/>
+    <workbookView xWindow="6180" yWindow="2355" windowWidth="21600" windowHeight="11160" xr2:uid="{4EF278E9-0480-487F-AE82-D1D1DBD956EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Biryani_Menu" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="100">
   <si>
     <t>Item Name</t>
   </si>
@@ -233,13 +233,100 @@
   </si>
   <si>
     <t>Kids Fries.</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/DKRtvJ7/800-6012d8a3a0807.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/4FddBW5/800-6012d8e670df3.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/2t7zHgL/800-6012d82e751c0.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/0QBLMr3/800-6012d9626749b.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/1XXDSmb/800-66392c99b094d.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/1rDv91n/800-66392dae99407.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/hBsYd8m/800-6012d1d6f1af8.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/P90SVMs/800-6012d21eefaf5.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/PZLbXzg/800-6012d13256a8b.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/3TJGtbR/800-60134f31a1f32.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/JmRZV7s/800-6012aab2c15a7.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/PZG8Njq/800-6012aa1e6fa36.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/PDgF2rJ/800-6012aa618cff2.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/zFxv5Ds/800-6012cf167d3bb.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/r01ytKq/800-6012ce8dd3461.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/t481pHP/800-6012ce5b80fc7.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/LPzxzRR/800-6012ce123334f.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/NL8T1TR/800-6012adc541a5b.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/Gd5PdtL/800-6012ae325a211.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/kDBKRbS/800-6012acac63175.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/h2t8vKN/800-6012ad30ba62d.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/bRrt19b/800-6012ad821225e.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/nRpWWtc/800-6012ac57acc78.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/fFJwgXM/800-6012a8d2ca653.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/KNkJ5nQ/800-6012a96d269da.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/KjyjT6F/800-6012a8655da02.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/nktXNQ3/800-6012a812af173.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/LdKwhWm/800-6012a6070a898.jpg</t>
+  </si>
+  <si>
+    <t>Image</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,6 +457,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -672,7 +767,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -715,11 +810,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -753,6 +850,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1093,13 +1191,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EAB86B-962C-4989-8B58-B102F2EA062D}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1109,8 +1209,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1120,8 +1223,11 @@
       <c r="C2">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1131,8 +1237,11 @@
       <c r="C3">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1142,8 +1251,11 @@
       <c r="C4">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1153,8 +1265,11 @@
       <c r="C5">
         <v>16.68</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1164,8 +1279,11 @@
       <c r="C6">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1175,8 +1293,11 @@
       <c r="C7">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1186,8 +1307,11 @@
       <c r="C8">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1197,8 +1321,11 @@
       <c r="C9">
         <v>16.68</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1208,8 +1335,11 @@
       <c r="C10">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1219,8 +1349,11 @@
       <c r="C11">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1230,8 +1363,11 @@
       <c r="C12">
         <v>16.68</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1241,8 +1377,11 @@
       <c r="C13">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1252,8 +1391,11 @@
       <c r="C14">
         <v>14.67</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1263,8 +1405,11 @@
       <c r="C15">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1274,8 +1419,11 @@
       <c r="C16">
         <v>16.68</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1285,8 +1433,11 @@
       <c r="C17">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1296,8 +1447,11 @@
       <c r="C18">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1307,8 +1461,11 @@
       <c r="C19">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1318,8 +1475,11 @@
       <c r="C20">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1329,8 +1489,11 @@
       <c r="C21">
         <v>16.68</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1340,8 +1503,11 @@
       <c r="C22">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1351,8 +1517,11 @@
       <c r="C23">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1362,8 +1531,11 @@
       <c r="C24">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -1373,8 +1545,11 @@
       <c r="C25">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1384,8 +1559,11 @@
       <c r="C26">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -1395,8 +1573,11 @@
       <c r="C27">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -1406,8 +1587,11 @@
       <c r="C28">
         <v>16.68</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -1417,8 +1601,11 @@
       <c r="C29">
         <v>16.68</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -1428,8 +1615,11 @@
       <c r="C30">
         <v>5.03</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -1439,8 +1629,11 @@
       <c r="C31">
         <v>5.03</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -1450,8 +1643,11 @@
       <c r="C32">
         <v>5.96</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -1461,8 +1657,11 @@
       <c r="C33">
         <v>6.63</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -1472,8 +1671,11 @@
       <c r="C34">
         <v>9.7100000000000009</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -1483,8 +1685,14 @@
       <c r="C35">
         <v>9.7100000000000009</v>
       </c>
+      <c r="D35" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{11A0EBB2-9FC3-4221-AF5B-F0D72A4F336B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I will test quick registration
</commit_message>
<xml_diff>
--- a/uploads/menu_file.xlsx
+++ b/uploads/menu_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmatr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F90374-943C-46CC-AF8F-D870DA54831D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99DA2FA-1E4D-4BCC-A898-5CC20756A525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6180" yWindow="2355" windowWidth="21600" windowHeight="11160" xr2:uid="{4EF278E9-0480-487F-AE82-D1D1DBD956EF}"/>
   </bookViews>
@@ -1194,7 +1194,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,7 +1643,7 @@
       <c r="C32">
         <v>5.96</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1692,6 +1692,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{11A0EBB2-9FC3-4221-AF5B-F0D72A4F336B}"/>
+    <hyperlink ref="D32" r:id="rId2" xr:uid="{3A3A61E9-6A78-4F13-8A25-42B814468648}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Testing voice agent order placement
</commit_message>
<xml_diff>
--- a/uploads/menu_file.xlsx
+++ b/uploads/menu_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmatr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99DA2FA-1E4D-4BCC-A898-5CC20756A525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BCF399-AE1A-4D61-90E2-27FD79F95B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="2355" windowWidth="21600" windowHeight="11160" xr2:uid="{4EF278E9-0480-487F-AE82-D1D1DBD956EF}"/>
+    <workbookView xWindow="5130" yWindow="2895" windowWidth="21600" windowHeight="11160" xr2:uid="{4EF278E9-0480-487F-AE82-D1D1DBD956EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Biryani_Menu" sheetId="1" r:id="rId1"/>
@@ -1194,7 +1194,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,7 +1293,7 @@
       <c r="C7">
         <v>15.34</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1321,7 +1321,7 @@
       <c r="C9">
         <v>16.68</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1693,6 +1693,8 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{11A0EBB2-9FC3-4221-AF5B-F0D72A4F336B}"/>
     <hyperlink ref="D32" r:id="rId2" xr:uid="{3A3A61E9-6A78-4F13-8A25-42B814468648}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{1E6160DD-B8AE-4EED-89DC-0878F6A73B1A}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{1FBA63AB-52A7-4D7A-81A3-151E23D13C56}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>